<commit_message>
massive reworking of the UI (it is now much cleaner), fixed rigid body performance issues, plus lots of other stuff
</commit_message>
<xml_diff>
--- a/ffxiv_mmd_tools_helper/data/joint.xlsx
+++ b/ffxiv_mmd_tools_helper/data/joint.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper_beta\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MMD\ffxiv_mmd_tools_helper\ffxiv_mmd_tools_helper\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90173F1A-D9AF-416F-9902-3ACA0152FA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBE0A3F-B050-42D0-AF8D-07FA9E0A83EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47040" yWindow="4035" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="3150" windowWidth="20820" windowHeight="14715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -279,7 +279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -287,9 +287,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D213BE9-EC88-43A5-B10E-7AC8A26A2FF6}">
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,49 +1110,25 @@
       <c r="A15" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" t="s">
         <v>36</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="7"/>
-      <c r="T15" s="7"/>
-      <c r="U15" s="7"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" t="s">
         <v>36</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="7"/>
-      <c r="T16" s="7"/>
-      <c r="U16" s="7"/>
-    </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -1165,20 +1138,8 @@
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="7"/>
-      <c r="T17" s="7"/>
-      <c r="U17" s="7"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>40</v>
       </c>
@@ -1188,20 +1149,8 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="7"/>
-      <c r="T18" s="7"/>
-      <c r="U18" s="7"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>41</v>
       </c>
@@ -1211,20 +1160,8 @@
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="P19" s="7"/>
-      <c r="Q19" s="7"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="7"/>
-      <c r="T19" s="7"/>
-      <c r="U19" s="7"/>
-    </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
@@ -1234,66 +1171,30 @@
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="P20" s="7"/>
-      <c r="Q20" s="7"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="7"/>
-      <c r="T20" s="7"/>
-      <c r="U20" s="7"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" t="s">
         <v>36</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="7"/>
-      <c r="P21" s="7"/>
-      <c r="Q21" s="7"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="7"/>
-      <c r="U21" s="7"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" t="s">
         <v>36</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="P22" s="7"/>
-      <c r="Q22" s="7"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="7"/>
-      <c r="T22" s="7"/>
-      <c r="U22" s="7"/>
-    </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>45</v>
       </c>
@@ -1303,20 +1204,8 @@
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="7"/>
-      <c r="P23" s="7"/>
-      <c r="Q23" s="7"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
         <v>46</v>
       </c>
@@ -1326,20 +1215,8 @@
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="7"/>
-      <c r="I24" s="7"/>
-      <c r="P24" s="7"/>
-      <c r="Q24" s="7"/>
-      <c r="R24" s="7"/>
-      <c r="S24" s="7"/>
-      <c r="T24" s="7"/>
-      <c r="U24" s="7"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>47</v>
       </c>
@@ -1349,20 +1226,8 @@
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="P25" s="7"/>
-      <c r="Q25" s="7"/>
-      <c r="R25" s="7"/>
-      <c r="S25" s="7"/>
-      <c r="T25" s="7"/>
-      <c r="U25" s="7"/>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>48</v>
       </c>
@@ -1372,66 +1237,30 @@
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7"/>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7"/>
-      <c r="T26" s="7"/>
-      <c r="U26" s="7"/>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" t="s">
         <v>36</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="P27" s="7"/>
-      <c r="Q27" s="7"/>
-      <c r="R27" s="7"/>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-      <c r="U27" s="7"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
@@ -1441,20 +1270,8 @@
       <c r="C29">
         <v>1</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
-      <c r="H29" s="7"/>
-      <c r="I29" s="7"/>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="7"/>
-      <c r="R29" s="7"/>
-      <c r="S29" s="7"/>
-      <c r="T29" s="7"/>
-      <c r="U29" s="7"/>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>52</v>
       </c>
@@ -1464,20 +1281,8 @@
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="7"/>
-      <c r="I30" s="7"/>
-      <c r="P30" s="7"/>
-      <c r="Q30" s="7"/>
-      <c r="R30" s="7"/>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>53</v>
       </c>
@@ -1487,20 +1292,8 @@
       <c r="C31">
         <v>1</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="7"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="7"/>
-      <c r="R31" s="7"/>
-      <c r="S31" s="7"/>
-      <c r="T31" s="7"/>
-      <c r="U31" s="7"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
         <v>54</v>
       </c>
@@ -1510,18 +1303,6 @@
       <c r="C32">
         <v>1</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="7"/>
-      <c r="H32" s="7"/>
-      <c r="I32" s="7"/>
-      <c r="P32" s="7"/>
-      <c r="Q32" s="7"/>
-      <c r="R32" s="7"/>
-      <c r="S32" s="7"/>
-      <c r="T32" s="7"/>
-      <c r="U32" s="7"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
@@ -1530,7 +1311,10 @@
       <c r="B33" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J33" s="7">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="J33">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K33">
@@ -1544,7 +1328,10 @@
       <c r="B34" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J34" s="7">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="J34">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K34">
@@ -1558,7 +1345,10 @@
       <c r="B35" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="7">
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="J35">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K35">
@@ -1572,7 +1362,10 @@
       <c r="B36" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="J36" s="7">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="J36">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K36">
@@ -1586,7 +1379,10 @@
       <c r="B37" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="J37" s="7">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="J37">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K37">
@@ -1600,7 +1396,10 @@
       <c r="B38" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J38" s="7">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="J38">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K38">
@@ -1608,13 +1407,16 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
+      <c r="A39" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="J39" s="7">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K39">
@@ -1622,13 +1424,16 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="J40" s="7">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="J40">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K40">
@@ -1636,13 +1441,16 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="9" t="s">
+      <c r="B41" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="J41" s="7">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="J41">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K41">
@@ -1650,13 +1458,16 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="J42" s="7">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="J42">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K42">
@@ -1664,13 +1475,16 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
+      <c r="A43" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J43" s="7">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="J43">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K43">
@@ -1678,13 +1492,16 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="8" t="s">
+      <c r="A44" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="B44" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J44" s="7">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="J44">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K44">
@@ -1692,13 +1509,16 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="8" t="s">
+      <c r="A45" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="J45" s="7">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="J45">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K45">
@@ -1706,13 +1526,16 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" s="9" t="s">
+      <c r="A46" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="9" t="s">
+      <c r="B46" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="J46" s="7">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="J46">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K46">
@@ -1720,13 +1543,16 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="A47" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B47" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="J47" s="7">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="J47">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K47">
@@ -1734,13 +1560,16 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="B48" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J48" s="7">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="J48">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K48">
@@ -1748,13 +1577,16 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="8" t="s">
+      <c r="A49" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="J49" s="7">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="J49">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K49">
@@ -1762,13 +1594,16 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="8" t="s">
+      <c r="A50" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="8" t="s">
+      <c r="B50" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J50" s="7">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="J50">
         <v>-5.3100000000000001E-2</v>
       </c>
       <c r="K50">
@@ -1797,50 +1632,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="4" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>